<commit_message>
adding full run for ZEV Jan R2-4 and modifying files for consistency in R2-4
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_J.PLAGGENBERG_01.10.20.xlsx
+++ b/bioSample/bioSample_J.PLAGGENBERG_01.10.20.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicaplaggenberg/Documents/rnaseq-database/bioSample/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B1B6EC-F2C9-F54E-A669-D4550A8FB575}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="2460" yWindow="460" windowWidth="16380" windowHeight="18280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,95 +27,76 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="20">
   <si>
-    <t xml:space="preserve">harvestDate</t>
+    <t>harvestDate</t>
   </si>
   <si>
-    <t xml:space="preserve">harvester</t>
+    <t>harvester</t>
   </si>
   <si>
-    <t xml:space="preserve">biosampleNumber</t>
+    <t>biosampleNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentDesign</t>
+    <t>experimentDesign</t>
   </si>
   <si>
-    <t xml:space="preserve">experimentObservations</t>
+    <t>experimentObservations</t>
   </si>
   <si>
-    <t xml:space="preserve">strain</t>
+    <t>strain</t>
   </si>
   <si>
-    <t xml:space="preserve">genotype</t>
+    <t>genotype</t>
   </si>
   <si>
-    <t xml:space="preserve">floodmedia</t>
+    <t>floodmedia</t>
   </si>
   <si>
-    <t xml:space="preserve">inductionDelay</t>
+    <t>inductionDelay</t>
   </si>
   <si>
-    <t xml:space="preserve">treatment</t>
+    <t>treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">timePoint</t>
+    <t>timePoint</t>
   </si>
   <si>
-    <t xml:space="preserve">replicate</t>
+    <t>replicate</t>
   </si>
   <si>
-    <t xml:space="preserve">01.10.20</t>
+    <t>01.10.20</t>
   </si>
   <si>
-    <t xml:space="preserve">J.PLAGGENBERG</t>
+    <t>J.PLAGGENBERG</t>
   </si>
   <si>
-    <t xml:space="preserve">ZEV_induction</t>
+    <t>ZEV_induction</t>
   </si>
   <si>
-    <t xml:space="preserve">Gal 4</t>
+    <t>SCGal</t>
   </si>
   <si>
-    <t xml:space="preserve">SCGal</t>
+    <t>EtOH</t>
   </si>
   <si>
-    <t xml:space="preserve">EtOH</t>
+    <t>Estradiol</t>
   </si>
   <si>
-    <t xml:space="preserve">Estradiol</t>
+    <t>RGT1</t>
   </si>
   <si>
-    <t xml:space="preserve">RGT1</t>
+    <t>GAL4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="10"/>
@@ -143,7 +129,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -155,7 +147,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -163,111 +155,362 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </cellStyleXfs>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J40" activeCellId="0" sqref="J40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="14.5"/>
+    <col min="1" max="2" width="14.5" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+    <col min="5" max="6" width="7" customWidth="1"/>
+    <col min="7" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="6.5" customWidth="1"/>
+    <col min="10" max="1025" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -319,14 +562,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -334,22 +577,22 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
+      <c r="G2" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="7">
+        <v>30</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="9" t="n">
+      <c r="K2" s="9">
         <v>-1</v>
       </c>
-      <c r="L2" s="9" t="n">
+      <c r="L2" s="9">
         <v>3</v>
       </c>
       <c r="M2" s="1"/>
@@ -367,14 +610,14 @@
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="10">
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -382,22 +625,22 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
+      <c r="G3" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" s="7">
         <v>30</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K3" s="9">
         <v>-1</v>
       </c>
-      <c r="L3" s="9" t="n">
+      <c r="L3" s="9">
         <v>3</v>
       </c>
       <c r="M3" s="1"/>
@@ -415,14 +658,14 @@
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="10">
         <v>3</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -430,22 +673,22 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
+      <c r="G4" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="7">
+        <v>30</v>
+      </c>
+      <c r="J4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L4" s="9" t="n">
+      <c r="K4" s="9">
+        <v>15</v>
+      </c>
+      <c r="L4" s="9">
         <v>3</v>
       </c>
       <c r="M4" s="1"/>
@@ -463,14 +706,14 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -478,22 +721,22 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
+      <c r="G5" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I5" s="7">
         <v>30</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L5" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K5" s="9">
+        <v>15</v>
+      </c>
+      <c r="L5" s="9">
         <v>3</v>
       </c>
       <c r="M5" s="1"/>
@@ -511,14 +754,14 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -526,22 +769,22 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
+      <c r="G6" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="7">
+        <v>30</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="9" t="n">
+      <c r="K6" s="9">
         <v>20</v>
       </c>
-      <c r="L6" s="9" t="n">
+      <c r="L6" s="9">
         <v>3</v>
       </c>
       <c r="M6" s="1"/>
@@ -559,14 +802,14 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="10">
         <v>6</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -574,22 +817,22 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
+      <c r="G7" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7">
         <v>30</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K7" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K7" s="9">
         <v>20</v>
       </c>
-      <c r="L7" s="9" t="n">
+      <c r="L7" s="9">
         <v>3</v>
       </c>
       <c r="M7" s="1"/>
@@ -607,14 +850,14 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="10">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -622,22 +865,22 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="5" t="s">
-        <v>15</v>
+      <c r="G8" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="7">
+        <v>30</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K8" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L8" s="9" t="n">
+      <c r="K8" s="7">
+        <v>30</v>
+      </c>
+      <c r="L8" s="9">
         <v>3</v>
       </c>
       <c r="M8" s="1"/>
@@ -655,14 +898,14 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -670,22 +913,22 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="5" t="s">
-        <v>15</v>
+      <c r="G9" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I9" s="7">
         <v>30</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L9" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K9" s="7">
+        <v>30</v>
+      </c>
+      <c r="L9" s="9">
         <v>3</v>
       </c>
       <c r="M9" s="1"/>
@@ -703,14 +946,14 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="3">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -718,22 +961,22 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="5" t="s">
-        <v>15</v>
+      <c r="G10" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="7">
+        <v>30</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K10" s="9" t="n">
+      <c r="K10" s="9">
         <v>90</v>
       </c>
-      <c r="L10" s="10" t="n">
+      <c r="L10" s="10">
         <v>3</v>
       </c>
       <c r="M10" s="1"/>
@@ -751,14 +994,14 @@
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="10">
         <v>10</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -766,22 +1009,22 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="5" t="s">
-        <v>15</v>
+      <c r="G11" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I11" s="7">
         <v>30</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K11" s="9">
         <v>90</v>
       </c>
-      <c r="L11" s="10" t="n">
+      <c r="L11" s="10">
         <v>3</v>
       </c>
       <c r="M11" s="1"/>
@@ -799,14 +1042,14 @@
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="10">
         <v>11</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -814,22 +1057,22 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="5" t="s">
-        <v>15</v>
+      <c r="G12" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="7">
+        <v>30</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K12" s="9" t="n">
+      <c r="K12" s="9">
         <v>-1</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="9">
         <v>4</v>
       </c>
       <c r="M12" s="1"/>
@@ -847,14 +1090,14 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="3">
         <v>12</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -862,22 +1105,22 @@
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="5" t="s">
-        <v>15</v>
+      <c r="G13" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I13" s="7">
         <v>30</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K13" s="9">
         <v>-1</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="9">
         <v>4</v>
       </c>
       <c r="M13" s="1"/>
@@ -895,14 +1138,14 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="3">
         <v>13</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -910,22 +1153,22 @@
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="5" t="s">
-        <v>15</v>
+      <c r="G14" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="7">
+        <v>30</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K14" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L14" s="9" t="n">
+      <c r="K14" s="9">
+        <v>15</v>
+      </c>
+      <c r="L14" s="9">
         <v>4</v>
       </c>
       <c r="M14" s="1"/>
@@ -943,14 +1186,14 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="10">
         <v>14</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -958,22 +1201,22 @@
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="5" t="s">
-        <v>15</v>
+      <c r="G15" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I15" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I15" s="7">
         <v>30</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L15" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9">
+        <v>15</v>
+      </c>
+      <c r="L15" s="9">
         <v>4</v>
       </c>
       <c r="M15" s="1"/>
@@ -991,14 +1234,14 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="10">
         <v>15</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1006,22 +1249,22 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="5" t="s">
-        <v>15</v>
+      <c r="G16" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="7">
+        <v>30</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I16" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K16" s="9" t="n">
+      <c r="K16" s="9">
         <v>20</v>
       </c>
-      <c r="L16" s="9" t="n">
+      <c r="L16" s="9">
         <v>4</v>
       </c>
       <c r="M16" s="1"/>
@@ -1039,14 +1282,14 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="3">
         <v>16</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -1054,22 +1297,22 @@
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="5" t="s">
-        <v>15</v>
+      <c r="G17" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I17" s="7">
         <v>30</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K17" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K17" s="9">
         <v>20</v>
       </c>
-      <c r="L17" s="9" t="n">
+      <c r="L17" s="9">
         <v>4</v>
       </c>
       <c r="M17" s="1"/>
@@ -1087,14 +1330,14 @@
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="3">
         <v>17</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1102,22 +1345,22 @@
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="5" t="s">
-        <v>15</v>
+      <c r="G18" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="7">
+        <v>30</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K18" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L18" s="9" t="n">
+      <c r="K18" s="7">
+        <v>30</v>
+      </c>
+      <c r="L18" s="9">
         <v>4</v>
       </c>
       <c r="M18" s="1"/>
@@ -1135,14 +1378,14 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="10">
         <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1150,22 +1393,22 @@
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="5" t="s">
-        <v>15</v>
+      <c r="G19" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I19" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I19" s="7">
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K19" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L19" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K19" s="7">
+        <v>30</v>
+      </c>
+      <c r="L19" s="9">
         <v>4</v>
       </c>
       <c r="M19" s="1"/>
@@ -1183,14 +1426,14 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="10">
         <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -1198,22 +1441,22 @@
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="5" t="s">
-        <v>15</v>
+      <c r="G20" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="7">
+        <v>30</v>
+      </c>
+      <c r="J20" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K20" s="9" t="n">
+      <c r="K20" s="9">
         <v>90</v>
       </c>
-      <c r="L20" s="10" t="n">
+      <c r="L20" s="10">
         <v>4</v>
       </c>
       <c r="M20" s="1"/>
@@ -1231,14 +1474,14 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="3">
         <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -1246,22 +1489,22 @@
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="5" t="s">
-        <v>15</v>
+      <c r="G21" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I21" s="7">
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K21" s="9">
         <v>90</v>
       </c>
-      <c r="L21" s="10" t="n">
+      <c r="L21" s="10">
         <v>4</v>
       </c>
       <c r="M21" s="1"/>
@@ -1279,14 +1522,14 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="3">
         <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -1295,21 +1538,21 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="7">
+        <v>30</v>
+      </c>
+      <c r="J22" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="9" t="n">
+      <c r="K22" s="9">
         <v>-1</v>
       </c>
-      <c r="L22" s="9" t="n">
+      <c r="L22" s="9">
         <v>3</v>
       </c>
       <c r="M22" s="1"/>
@@ -1327,14 +1570,14 @@
       <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="10">
         <v>22</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -1343,21 +1586,21 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I23" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I23" s="7">
         <v>30</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K23" s="9">
         <v>-1</v>
       </c>
-      <c r="L23" s="9" t="n">
+      <c r="L23" s="9">
         <v>3</v>
       </c>
       <c r="M23" s="1"/>
@@ -1375,14 +1618,14 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="10">
         <v>23</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -1391,21 +1634,21 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="7">
+        <v>30</v>
+      </c>
+      <c r="J24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K24" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L24" s="9" t="n">
+      <c r="K24" s="9">
+        <v>15</v>
+      </c>
+      <c r="L24" s="9">
         <v>3</v>
       </c>
       <c r="M24" s="1"/>
@@ -1423,14 +1666,14 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="3">
         <v>24</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -1439,21 +1682,21 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I25" s="7">
         <v>30</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K25" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L25" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K25" s="9">
+        <v>15</v>
+      </c>
+      <c r="L25" s="9">
         <v>3</v>
       </c>
       <c r="M25" s="1"/>
@@ -1471,14 +1714,14 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="3" t="n">
+      <c r="C26" s="3">
         <v>25</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -1487,21 +1730,21 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="7">
+        <v>30</v>
+      </c>
+      <c r="J26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I26" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K26" s="9" t="n">
+      <c r="K26" s="9">
         <v>20</v>
       </c>
-      <c r="L26" s="9" t="n">
+      <c r="L26" s="9">
         <v>3</v>
       </c>
       <c r="M26" s="1"/>
@@ -1519,14 +1762,14 @@
       <c r="Y26" s="1"/>
       <c r="Z26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="10">
         <v>26</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -1535,21 +1778,21 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I27" s="7">
         <v>30</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K27" s="9">
         <v>20</v>
       </c>
-      <c r="L27" s="9" t="n">
+      <c r="L27" s="9">
         <v>3</v>
       </c>
       <c r="M27" s="1"/>
@@ -1567,14 +1810,14 @@
       <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="10">
         <v>27</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -1583,21 +1826,21 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="7">
+        <v>30</v>
+      </c>
+      <c r="J28" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I28" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L28" s="9" t="n">
+      <c r="K28" s="7">
+        <v>30</v>
+      </c>
+      <c r="L28" s="9">
         <v>3</v>
       </c>
       <c r="M28" s="1"/>
@@ -1615,14 +1858,14 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="3">
         <v>28</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -1631,21 +1874,21 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I29" s="7">
         <v>30</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K29" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L29" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K29" s="7">
+        <v>30</v>
+      </c>
+      <c r="L29" s="9">
         <v>3</v>
       </c>
       <c r="M29" s="1"/>
@@ -1663,14 +1906,14 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="3" t="n">
+      <c r="C30" s="3">
         <v>29</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -1679,21 +1922,21 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H30" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="7">
+        <v>30</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I30" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="9" t="n">
+      <c r="K30" s="9">
         <v>90</v>
       </c>
-      <c r="L30" s="10" t="n">
+      <c r="L30" s="10">
         <v>3</v>
       </c>
       <c r="M30" s="1"/>
@@ -1711,14 +1954,14 @@
       <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="10" t="n">
+      <c r="C31" s="10">
         <v>30</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -1727,21 +1970,21 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I31" s="7">
         <v>30</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K31" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K31" s="9">
         <v>90</v>
       </c>
-      <c r="L31" s="10" t="n">
+      <c r="L31" s="10">
         <v>3</v>
       </c>
       <c r="M31" s="1"/>
@@ -1759,14 +2002,14 @@
       <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="10" t="n">
+      <c r="C32" s="10">
         <v>31</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -1775,21 +2018,21 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="7">
+        <v>30</v>
+      </c>
+      <c r="J32" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K32" s="9" t="n">
+      <c r="K32" s="9">
         <v>-1</v>
       </c>
-      <c r="L32" s="9" t="n">
+      <c r="L32" s="9">
         <v>4</v>
       </c>
       <c r="M32" s="1"/>
@@ -1807,14 +2050,14 @@
       <c r="Y32" s="1"/>
       <c r="Z32" s="1"/>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="3">
         <v>32</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -1823,21 +2066,21 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I33" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I33" s="7">
         <v>30</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K33" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K33" s="9">
         <v>-1</v>
       </c>
-      <c r="L33" s="9" t="n">
+      <c r="L33" s="9">
         <v>4</v>
       </c>
       <c r="M33" s="1"/>
@@ -1855,14 +2098,14 @@
       <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="3">
         <v>33</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -1871,21 +2114,21 @@
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="7">
+        <v>30</v>
+      </c>
+      <c r="J34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I34" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K34" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L34" s="9" t="n">
+      <c r="K34" s="9">
+        <v>15</v>
+      </c>
+      <c r="L34" s="9">
         <v>4</v>
       </c>
       <c r="M34" s="1"/>
@@ -1903,14 +2146,14 @@
       <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="10" t="n">
+      <c r="C35" s="10">
         <v>34</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -1919,21 +2162,21 @@
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I35" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I35" s="7">
         <v>30</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K35" s="9" t="n">
-        <v>15</v>
-      </c>
-      <c r="L35" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K35" s="9">
+        <v>15</v>
+      </c>
+      <c r="L35" s="9">
         <v>4</v>
       </c>
       <c r="M35" s="1"/>
@@ -1951,14 +2194,14 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="10" t="n">
+      <c r="C36" s="10">
         <v>35</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -1967,21 +2210,21 @@
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="7">
+        <v>30</v>
+      </c>
+      <c r="J36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I36" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K36" s="9" t="n">
+      <c r="K36" s="9">
         <v>20</v>
       </c>
-      <c r="L36" s="9" t="n">
+      <c r="L36" s="9">
         <v>4</v>
       </c>
       <c r="M36" s="1"/>
@@ -1999,14 +2242,14 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="3">
         <v>36</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -2015,21 +2258,21 @@
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I37" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I37" s="7">
         <v>30</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K37" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K37" s="9">
         <v>20</v>
       </c>
-      <c r="L37" s="9" t="n">
+      <c r="L37" s="9">
         <v>4</v>
       </c>
       <c r="M37" s="1"/>
@@ -2047,14 +2290,14 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="3">
         <v>37</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -2063,21 +2306,21 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H38" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I38" s="7">
+        <v>30</v>
+      </c>
+      <c r="J38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I38" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J38" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K38" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L38" s="9" t="n">
+      <c r="K38" s="7">
+        <v>30</v>
+      </c>
+      <c r="L38" s="9">
         <v>4</v>
       </c>
       <c r="M38" s="1"/>
@@ -2095,14 +2338,14 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="10" t="n">
+      <c r="C39" s="10">
         <v>38</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -2111,21 +2354,21 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I39" s="7">
         <v>30</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K39" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="L39" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K39" s="7">
+        <v>30</v>
+      </c>
+      <c r="L39" s="9">
         <v>4</v>
       </c>
       <c r="M39" s="1"/>
@@ -2143,14 +2386,14 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="10" t="n">
+      <c r="C40" s="10">
         <v>39</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -2159,21 +2402,21 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H40" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="7">
+        <v>30</v>
+      </c>
+      <c r="J40" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I40" s="7" t="n">
-        <v>30</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="9" t="n">
+      <c r="K40" s="9">
         <v>90</v>
       </c>
-      <c r="L40" s="10" t="n">
+      <c r="L40" s="10">
         <v>4</v>
       </c>
       <c r="M40" s="1"/>
@@ -2191,14 +2434,14 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="3">
         <v>40</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -2207,21 +2450,21 @@
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="7" t="n">
+        <v>15</v>
+      </c>
+      <c r="I41" s="7">
         <v>30</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K41" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="K41" s="9">
         <v>90</v>
       </c>
-      <c r="L41" s="10" t="n">
+      <c r="L41" s="10">
         <v>4</v>
       </c>
       <c r="M41" s="1"/>
@@ -2240,12 +2483,7 @@
       <c r="Z41" s="1"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>